<commit_message>
Construct leakage function for one bottle, apply to thermal hydrolysis
</commit_message>
<xml_diff>
--- a/experiments/thermal hydrolysis/Leakage.xlsx
+++ b/experiments/thermal hydrolysis/Leakage.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Leakage calculation</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>tot.mass.loss</t>
+  </si>
+  <si>
+    <t>interval</t>
   </si>
 </sst>
 </file>
@@ -392,30 +395,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I7"/>
+  <dimension ref="B2:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -423,96 +427,103 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
-        <v>385.27</v>
-      </c>
       <c r="E5">
         <v>385.27</v>
       </c>
       <c r="F5">
-        <f>E5-D5</f>
+        <v>385.27</v>
+      </c>
+      <c r="G5">
+        <f>E5-F5</f>
         <v>0</v>
       </c>
-      <c r="H5">
-        <f>F5+G5</f>
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>0.90690000000000004</v>
       </c>
       <c r="D6">
+        <f>C6-C5</f>
+        <v>0.90690000000000004</v>
+      </c>
+      <c r="E6">
         <v>385.26</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>385.04</v>
       </c>
-      <c r="F6">
-        <f t="shared" ref="F6:F7" si="0">E6-D6</f>
-        <v>-0.21999999999997044</v>
-      </c>
       <c r="G6">
-        <f>E5-D6</f>
+        <f>E6-F6</f>
+        <v>0.21999999999997044</v>
+      </c>
+      <c r="H6">
+        <f>F5-E6</f>
         <v>9.9999999999909051E-3</v>
       </c>
-      <c r="H6">
-        <f t="shared" ref="H6:H7" si="1">F6+G6</f>
-        <v>-0.20999999999997954</v>
+      <c r="I6">
+        <f>F5-F6</f>
+        <v>0.22999999999996135</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>2.0381</v>
       </c>
       <c r="D7">
+        <f>C7-C6</f>
+        <v>1.1312</v>
+      </c>
+      <c r="E7">
         <v>385.04</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>384.8</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>-0.24000000000000909</v>
-      </c>
       <c r="G7">
-        <f>E6-D7</f>
+        <f>E7-F7</f>
+        <v>0.24000000000000909</v>
+      </c>
+      <c r="H7">
+        <f>F6-E7</f>
         <v>0</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="1"/>
-        <v>-0.24000000000000909</v>
+      <c r="I7">
+        <f>F6-F7</f>
+        <v>0.24000000000000909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>